<commit_message>
fixe json file edit excel reader
</commit_message>
<xml_diff>
--- a/server/exe1.xlsx
+++ b/server/exe1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\tp_si\project\project-si\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B90676-E434-4279-BEE5-0CC4963371E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35DB69B-83C6-4A71-922B-55A8536C7E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{9E8DD66C-66A2-4FAF-BDE8-9647EE6088AA}"/>
   </bookViews>
@@ -54,19 +54,19 @@
     <t>djoudi</t>
   </si>
   <si>
-    <t>telephoneClient</t>
-  </si>
-  <si>
-    <t>creditClient</t>
-  </si>
-  <si>
-    <t>prenomClient</t>
-  </si>
-  <si>
-    <t>adresseClient</t>
-  </si>
-  <si>
-    <t>nomClient</t>
+    <t>Nom_fournisseur</t>
+  </si>
+  <si>
+    <t>Prenom_fournisseur</t>
+  </si>
+  <si>
+    <t>adresse_fournisseur</t>
+  </si>
+  <si>
+    <t>telephone_fournisseur</t>
+  </si>
+  <si>
+    <t>solde_fournisseur</t>
   </si>
 </sst>
 </file>
@@ -439,26 +439,26 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -474,6 +474,9 @@
       <c r="D2">
         <v>23244</v>
       </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -488,6 +491,9 @@
       <c r="D3">
         <v>3232</v>
       </c>
+      <c r="E3">
+        <v>31231</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
@@ -501,6 +507,9 @@
       </c>
       <c r="D4">
         <v>3232</v>
+      </c>
+      <c r="E4">
+        <v>21312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>